<commit_message>
Update Opinosis Human Eval to ensure consistent format
</commit_message>
<xml_diff>
--- a/human_evaluation/For_Evaluator_IDHERE_Opin.xlsx
+++ b/human_evaluation/For_Evaluator_IDHERE_Opin.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="460" windowWidth="25600" windowHeight="20020" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Bestwestern-Parking" sheetId="7" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>the font is clear and adjustable in size . while they may not reproduce the look of a printed page, applications for these devices, such as ereader, do offer a variety of font types, background colors, and page turning mechanisms,</t>
   </si>
   <si>
-    <t>Easy to use and accurate. Accurate pois.</t>
-  </si>
-  <si>
     <t>would arrive home . 0 out of 5 stars gps navigator doesn't navigate accurately on a straight road . i was familiar with the streets and only used the nuvi to get an accurate arrival time estimate . but after that it is very easy and is very,</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>i've i've used other gps units, as well as gps built into cars and to this day nothing beats the accuracy of a garmin gps . i've used other gps units, as well as gps built into cars and to this day nothing beats the accuracy of a garmin gps .</t>
   </si>
   <si>
-    <t>The font is adjustable and easy to change</t>
-  </si>
-  <si>
     <t>Bestwestern Inn, San Fransisco: Parking</t>
   </si>
   <si>
@@ -139,18 +133,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Parking was expensive but I think this is common for San Fran . there is a fee for parking but well worth it seeing no where to park if you do have a car . The parking was free, which was great, and the hotel was conveniently located for public transport, and local attractions .As for in, and, out parking, I have seen a lot of San Francisco with no car at all . They have a parking garage, but they make you leave your vehicle for them to park   and then if you want to take a drive later, you have to wait for the staff to get it . There is no real parking space, so I had to pull up in front of the hotel in a small space .There was valet parking at a cost of $42 . Rooms are very comfortable and we were charged $15 for parking our motorcycle in the garage . Our ONLY complaint was one doorman valet wasn't thrilled about us parking the car at the front  Parking is easier then you might realize . There is a parking ramp across the street that is MUCH cheaper then hotel parking . Our room rate was all in order ñ weíd booked a TravelZoo special, and the front desk had the right rate, and the right parking discount . Of course you have the added thrill of paying over $40 a night for parking and whatever your chiropractor bill is when you are done with the beds .I found a great mid week deal that included a discount on parking .On the other hand, the valet parking attendant bell people were very friendly .Parking is expensive, Rooms are on the small side . However, parking is $30 night and valet only, which becomes a pain .Only other downer was $38 per night for valet parking .room was quiet, clean with good beds but very very smallnot a cheap hotelvalit parking was to much expencive but oke its the location Parking is crazy expensive, we drove up from LA so we had a car ,  but otherwise, you really don't need it . Parking is expensive   and everything is very much within walking distance . Valet parking is, in my view, unreasonably high at $38 per night, but again we knew this before we arrived so can't really complain . As most hotels in the city, parking is expensive so unless you really need a vehicle itís cheaper to just buy a MUNI Passport during your stay . The hotel does have parking, but it is expensive and hard to get around the city while driving . The parking was steep  , so if I had to do it again I would have parked 1 2 block north for about half of that . Parking at $45 a night was outrageous, but probably worth it to keep your car safe . We did not have a car, hotel parking is expensive . The valet parking was very convenient and seemed secure as it is attached to the hotel . A lot of hotel parking garages lots are not on the same premises as the hotel in the area . First, the biggest &amp;quot gotcha&amp;quot  is the mandatory valet parking . Not trying to bad mouth the Tuscan, it is a nice place to stay, and if you're not put off by the valet parking, you shouldn't be too disappointed . Valet parking for $40 per night seems a bit steep,but at least the service was efficient and quick . The prize for vallet parking is steep but I think you can expect that anywhere you go in San Francisco . Valet parking was $45 per night with tax, but that includes in and out privileges and my car was there whenever I needed it . Watch out for steep parking rates of about $45 per night . This total includes the taxes and tips for mandatory valet parking .Aside from the parking rate, you won't be disappointed . The other thing that I found disappointing was I can't remember the exact details but something like the charge they quote for parking   was even more than that because there was some sort of a tax . Onsite parking is available . I called before we ever arrived to inquire about it and was told that parking was no problem at all . I guess calling to inquire about parking while giving them our name and reservation dates didn't warrant the clerk to inform us that we should make a reservation for our car also . Valet parking is provided at $36 day which was, I thought, excessive .Walgreens has same souvenirs the airport shops do for 1 2 $Do not rent a car, waste of time, money,   no parking !The valet parking was overpriced, the service was terrible, and the coffe was cold . At the hotel, it is valet only parking . Check for Internet deals and don't pay for their parking . I do think that if you are staying at a hotel you should not have to pay for parking .The hotel, located a few blocks from Fisherman's Wharf as well as Ghiardelli Square, has a nice Italian theme that carries into the lobby as well as the uniforms for the parking valets . Speaking of parking, you're going to have to pay and it's going to have to be valet service, as there are no free self park lots that are part of the hotel . Not only is it pricey at $36 day, but having nothing but valet parking means you have no access to your car unless you have one of the valets fetch it from the lot for you . Although our room was indeed non, smoking   and we had a king size bed we ended up on the 3rd floor and our room, facing Mason Street, overlooked a concrete multi, story parking lot although if you stood at the window you could see the Coit Tower which was a nicer view ! Several have mentioned the charge for parking . It really does save if you can get a deal with free parking, but the fee is not out of line . Valet parking was $36 a day, but we're not complaining because other SF wharf hotels have charged us a similar fee even without the valet service . Another irritant was the crazy parking fees for the hotel . They do a good job and are a heck of a lot cheaper than a cab and you wonít have to mess with the parking fees . When I got a GREAT deal $99 INCLUDING parking !The great thing for us was the free parking . Normally parking is $36 a night so getting that thrown in was a fantastic steal .We stayed at the BW Tuscan Inn only because they were offering a great winter deal , $99 for a room with king, size bed and free parking   . Overall, we would recommend this place to friends, especially if they are able to get a good discount and free parking . Nice rooms, a bit on the smaller side, but parking right at the hotel . staff were helpful although the valet parking and the laundry costs were extremely expensive . They allowed this, so we only had to pay the regular parking fee of the hotel . Way too much money to pay for parking, but that is the way it is in San Francisco . You don't need a car because parking is a nightmare .all these hotels charge parking fees . Parking at the hotel is expensive at $32 plus tax per night but the up side is that you have in out privilages .Parking in the city is a royal pain ! Although the parking charge is steep, it seems to be the market price in San Francisco, or as the locals like to call it : I notice on other reviews the high cost of parking which we didn't have to consider as we were advised you do not need a car to get around SF, and this is quite true . All in all, the location was perfect ,  a short walk to the cable cars or bus lines, a Safeway grocery and Walgreens drugs is across the street in a parking garage, type mall, and there are small places to eat breakfast nearby plus an IHOP a few blocks over . Parking at the hotel was a hefty $32 per day with unlimited in and out privileges . Parking is an issue in SF so either pay the $30 . In addition, the valet parking is apparently handled by an outside contractor, and turned out to be considerably more expensive than we had been told ,  $35 day ,  which seemed very high . Because of the exhorbitant $29 valet parking fee, we only rented a car for Sonoma and Napa for one day . You'll be having fun while some other poor sod is looking for a parking space that isn't there .30 am, we discovered that the parking garage next door   would not be open until 7 ,  7 : I thought the $29 per day parking was ridiculous, but I hear that's the standard in SF .Upon arriving, there was a very long and confusing to do with the valet parking ,  we hadn't gotten our luggage out of th car and the valet wanted the keys . There was a fee of $29 per day for the parking . Valet parking attendant was no better . paid $161 plus tax along with a $20 parking fee .As far as parking is concerned, we were shell, shocked at what most of the hotels charge for parkingóup to $40 night . The Tuscan is $29 night, but if you search for a package rate on their web site, you may get parking included in your room rate . And, conveniently, there is a Safeway and a drug store hidden in the parking garage across the street . We didnt have or need a car so we didnt have to deal with parking a car I believe it is $30 a day, ,  par for the city . It is located 2 blocks from the wharf which was outstanding considering parking is hard to come by .Note to those with a car, overnight valet parking is $26 but right next door the car park is $15 and it takes about 30 seconds to get from your car back to the hotel ,  why pay $26 ? Parking was $26 day ,  free valet with on and off priv . Make sure you realize that you pay for parking .00 for valet parking, but that was okay . I was aupset, since my $89 night room had gone to $138 night between the parking   and the pet charge . We didn't pull our car out of the parking garage the whole time we were there . Parking is not cheap, check before you go . Parking was only $10 with AAA rate . Hotel parking   is now $23 a night .</t>
-  </si>
-  <si>
-    <t>The parking is expensive and steep.</t>
-  </si>
-  <si>
-    <t>The food was excellent, good and delicious. Very good selection of food.</t>
-  </si>
-  <si>
-    <t>Free wine receiption in evening. Free coffee and biscotti and wine.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas mileage has been disappointing. Gas mileage is horrible and not good. </t>
   </si>
   <si>
     <t>2007 Toyota Camry: Gas Mileage</t>
@@ -215,6 +197,24 @@
   </si>
   <si>
     <t xml:space="preserve">The wine reception is a great idea as it is nice to meet other travellers and great having access to the free Internet access in our room . They also have a computer available with free internet which is a nice bonus but I didn't find that out till the day before we left but was still able to get on there to check our flight to Vegas the next day . The service was good, very friendly staff and we loved the free wine reception each night . has free wireless and help you with transportation needs . The nightly free wine tasting from 5 ,  6 pm is a brilliant idea and gets guests together to socialise witheach other . They have a happy hour where you have a couple offree drinks between 5 and 6 and this gives you a chance to meet other travellers . free wifi and happy hour wine every afternoon ! The parking was free, which was great, and the hotel was conveniently located for public transport, and local attractions . We were also told of the free wine reception at 5pm, great idea as it meant you could chat to your fellow guests . Free internet access and Happy Hour every afternoon . As said before, the free wine reception in the evening is Two Buck Chuck, drinkable, but certainly not anything to write home about . The free wine tasting every night was a wonderful extra and welcomed relaxment in between a long day of sightseeing and evenings out . That and also the free coffee and tea   every morning were little extras that we felt made you feel like a welcomed guest and that they are going out of their way to make the hotel special . Free internet in the lobby but none of any sort in the rooms .The hotel lobby was lovely, real fire, large comfy chairs and free internet access in the corner . There is a concierge, also free wine and appetizers in the afternoon .00 for an adult with free entrance for shildren , ,  we were both fascinated for nearly two hours and it was not crowded . We went down for the free wine reception, and had a great time .The hotel has one computer   available with free internet . And free wifi throughout the hotel which worked flawlessly . The room also has free wireless which I've read other hotels nearby don't . Free Wifi in your room, and the free wine reception in the evenings was great . The free happy hour really made the visit extra special ,  we met so many wonderful people during our 7 day stay this way . I personally appreciated the free internet service in the hotel . Free internet and a computer for use in the lobby was helpful . The manager's cocktail hour was a nice touch, and the free coffee in the morning was also nice though I had to ask both mornings for hot chocolate to be brought out for the kids, and the advertised biscotti was no where to be found . I didn't get to take advantage of the free coffee in the morning, but my husband and I did go to the 5pm, 6pm cocktail hour, which we enjoyed . Coffee and biscotti were available in reception every morning free of charge or if you preferred, there was a restaurant in the hotel that served breakfast or a Starbucks round the corner .This hotel offers a lot ,  a great location, great staff, free wine tastings and morning coffee . I booked a standard king room and was up graded to a premier king free of charge upon our arrival .This is a hassle, free place to stay with a dog . The hotel had free coffee and drinks everyday and free access to wireless internet . Free coffee and biscotti in the morning helped get the GF out of bed .00 found most other places closing so it was Hobsons choiceThe best part of the stay were the free wine and eats in the lounge arond 17 :The free wine and nibbles served between 5pm and 6pm were a lovely touch . We did however take advantage of the free coffee and biscotti that was offered every morning in the lobby .No bar as such in the hotel but they have free wine tasting every day at 5p .The free wine beer and coffee hot chocolate biscotti is a wonderful touch and we took full advantage of it . The late afternoon free wine reception was a really nice touch and we enjoyed this very much . Although we didn't use it, there was free Internet access in the room .l also enjoyed the morning coffee in the lobby and the free wine . The lobby area was really pleasant and the free wine   gets you talking to other guests .The free morning hot cocoa and coffee was nice before our daily excursions . The afternoon wine and cheese was a nice bonus as was the free Internet . We were surprised and delighted when, on arrival, we were given tokens for free continental breakasts . The reception area is compact and during the free evening </t>
+  </si>
+  <si>
+    <t>easy to use and accurate . accurate pois .</t>
+  </si>
+  <si>
+    <t>the parking is expensive and steep .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gas mileage has been disappointing . gas mileage is horrible and not good .  </t>
+  </si>
+  <si>
+    <t>free wine receiption in evening . free coffee and biscotti and wine .</t>
+  </si>
+  <si>
+    <t>the food was excellent, good and delicious . very good selection of food .</t>
+  </si>
+  <si>
+    <t>the font is adjustable and easy to change</t>
   </si>
 </sst>
 </file>
@@ -786,9 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -808,7 +806,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
@@ -821,7 +819,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -843,22 +841,22 @@
         <v>0</v>
       </c>
       <c r="C5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="18" t="s">
+      <c r="H5" s="19" t="s">
         <v>25</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -950,9 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -972,7 +968,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
@@ -985,7 +981,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -1007,22 +1003,22 @@
         <v>0</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -1114,9 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1136,7 +1130,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
@@ -1149,7 +1143,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -1171,22 +1165,22 @@
         <v>0</v>
       </c>
       <c r="C5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>48</v>
-      </c>
       <c r="G5" s="17" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -1278,9 +1272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1300,7 +1292,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
@@ -1313,7 +1305,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -1335,22 +1327,22 @@
         <v>0</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -1442,9 +1434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1502,7 +1492,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>15</v>
@@ -1606,9 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1666,19 +1654,19 @@
         <v>13</v>
       </c>
       <c r="D5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="18" t="s">
+      <c r="G5" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>19</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">

</xml_diff>